<commit_message>
parte neals y jj - entregable2
</commit_message>
<xml_diff>
--- a/G3-Tablero Kanban_ Calidad y Mejora Continua.xlsx
+++ b/G3-Tablero Kanban_ Calidad y Mejora Continua.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\kanban_continua-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\TECSUP\AÑO 2 - SEMESTRE 3\MejContinua\Kanban\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C671AD6C-721C-468B-82B6-BA174CDA8BFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE384D75-C02B-442F-AD0E-E40A465B4DB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15696" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATOS" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,8 @@
     <customWorkbookView name="Filtro 1" guid="{6D37D4BD-4770-4892-8DF3-C2DF475ACC4D}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <pivotCaches>
-    <pivotCache cacheId="73" r:id="rId5"/>
-    <pivotCache cacheId="89" r:id="rId6"/>
+    <pivotCache cacheId="29" r:id="rId5"/>
+    <pivotCache cacheId="37" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -873,7 +873,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -948,50 +948,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -999,9 +958,6 @@
     </xf>
     <xf numFmtId="2" fontId="15" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1020,14 +976,10 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="10" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1043,6 +995,52 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1206,8 +1204,8 @@
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2857500" cy="2857500"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Situacion_1">
@@ -1230,7 +1228,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1279,8 +1277,8 @@
       <xdr:rowOff>62865</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2857500" cy="2857500"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Responsable_2">
@@ -1303,7 +1301,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1352,8 +1350,8 @@
       <xdr:rowOff>198120</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2857500" cy="2857500"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Prioridad_3">
@@ -1376,7 +1374,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1421,7 +1419,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="ASUS" refreshedDate="45053.734139120374" refreshedVersion="6" recordCount="26" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HP" refreshedDate="45053.872638310182" refreshedVersion="6" recordCount="26" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B9:N35" sheet="DATOS"/>
   </cacheSource>
@@ -1540,9 +1538,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Progreso" numFmtId="9">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1" count="3">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="1" count="4">
         <n v="1"/>
         <n v="0"/>
+        <n v="0.33300000000000002"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1559,7 +1558,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="ASUS" refreshedDate="45053.734223726853" refreshedVersion="6" recordCount="25" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HP" refreshedDate="45053.872885879631" refreshedVersion="6" recordCount="25" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B9:N34" sheet="DATOS"/>
   </cacheSource>
@@ -1670,7 +1669,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Progreso" numFmtId="9">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="1"/>
     </cacheField>
     <cacheField name="Trabajo_Hrs" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="2"/>
@@ -1863,7 +1862,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
+    <x v="2"/>
     <n v="2"/>
   </r>
   <r>
@@ -1874,11 +1873,11 @@
     <x v="3"/>
     <x v="0"/>
     <d v="2023-04-12T00:00:00"/>
-    <d v="2023-05-07T00:00:00"/>
+    <d v="2023-04-12T00:00:00"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
   </r>
   <r>
@@ -1889,11 +1888,11 @@
     <x v="4"/>
     <x v="0"/>
     <d v="2023-04-12T00:00:00"/>
-    <d v="2023-05-07T00:00:00"/>
+    <d v="2023-04-12T00:00:00"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
   </r>
   <r>
@@ -2073,7 +2072,7 @@
     <x v="4"/>
     <x v="2"/>
     <x v="3"/>
-    <x v="2"/>
+    <x v="3"/>
     <m/>
   </r>
 </pivotCacheRecords>
@@ -2258,7 +2257,7 @@
     <x v="1"/>
     <x v="1"/>
     <x v="1"/>
-    <n v="0"/>
+    <n v="0.33300000000000002"/>
     <n v="2"/>
   </r>
   <r>
@@ -2269,11 +2268,11 @@
     <x v="3"/>
     <x v="0"/>
     <d v="2023-04-12T00:00:00"/>
-    <d v="2023-05-07T00:00:00"/>
+    <d v="2023-04-12T00:00:00"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
     <n v="2"/>
   </r>
   <r>
@@ -2284,11 +2283,11 @@
     <x v="4"/>
     <x v="0"/>
     <d v="2023-04-12T00:00:00"/>
-    <d v="2023-05-07T00:00:00"/>
+    <d v="2023-04-12T00:00:00"/>
     <x v="1"/>
     <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
+    <x v="0"/>
+    <n v="1"/>
     <n v="2"/>
   </r>
   <r>
@@ -2460,7 +2459,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="DASHBOARD" cacheId="73" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="DASHBOARD" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="B27:J52" firstHeaderRow="1" firstDataRow="1" firstDataCol="8"/>
   <pivotFields count="13">
     <pivotField name="Tipo" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -2569,10 +2568,11 @@
       </items>
     </pivotField>
     <pivotField name="Progreso" axis="axisRow" dataField="1" compact="0" numFmtId="9" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="4">
+      <items count="5">
         <item x="1"/>
+        <item x="2"/>
         <item x="0"/>
-        <item x="2"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2597,7 +2597,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="8"/>
@@ -2606,7 +2606,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="11"/>
@@ -2615,7 +2615,7 @@
       <x v="2"/>
       <x/>
       <x/>
-      <x/>
+      <x v="1"/>
     </i>
     <i r="1">
       <x v="14"/>
@@ -2714,7 +2714,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="1"/>
@@ -2723,7 +2723,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="2"/>
@@ -2732,7 +2732,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="3"/>
@@ -2741,7 +2741,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="4"/>
@@ -2750,7 +2750,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="5"/>
@@ -2759,7 +2759,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="6"/>
@@ -2768,7 +2768,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="9"/>
@@ -2777,7 +2777,7 @@
       <x v="1"/>
       <x v="1"/>
       <x v="1"/>
-      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="10"/>
@@ -2794,8 +2794,8 @@
       <x/>
       <x v="2"/>
       <x/>
-      <x/>
-      <x/>
+      <x v="1"/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="13"/>
@@ -2803,8 +2803,8 @@
       <x/>
       <x v="2"/>
       <x/>
-      <x/>
-      <x/>
+      <x v="1"/>
+      <x v="2"/>
     </i>
   </rowItems>
   <colItems count="1">
@@ -2823,7 +2823,219 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="KANBAN" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="KANBAN 3" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+  <location ref="M10:Q22" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="13">
+    <pivotField name="Tipo" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="Item ID" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="Tareas" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="39">
+        <item x="0"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="23"/>
+        <item m="1" x="25"/>
+        <item x="22"/>
+        <item x="20"/>
+        <item m="1" x="35"/>
+        <item m="1" x="31"/>
+        <item m="1" x="28"/>
+        <item m="1" x="27"/>
+        <item m="1" x="30"/>
+        <item m="1" x="32"/>
+        <item m="1" x="38"/>
+        <item m="1" x="34"/>
+        <item m="1" x="37"/>
+        <item m="1" x="33"/>
+        <item m="1" x="26"/>
+        <item x="21"/>
+        <item x="24"/>
+        <item m="1" x="29"/>
+        <item m="1" x="36"/>
+      </items>
+    </pivotField>
+    <pivotField name="Predecesor" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="Responsable" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="14">
+        <item m="1" x="11"/>
+        <item m="1" x="13"/>
+        <item m="1" x="9"/>
+        <item m="1" x="7"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item m="1" x="12"/>
+        <item m="1" x="8"/>
+        <item x="3"/>
+        <item m="1" x="10"/>
+        <item x="1"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="6"/>
+      </items>
+    </pivotField>
+    <pivotField name="Prioridad" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+      </items>
+    </pivotField>
+    <pivotField name="Inicio" compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="Fin" compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="Vencimiento" axis="axisRow" compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
+      <items count="5">
+        <item m="1" x="4"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+      </items>
+    </pivotField>
+    <pivotField name="Situacion" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Estado" axis="axisPage" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Progreso" compact="0" numFmtId="9" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="Trabajo_Hrs" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="5">
+    <field x="2"/>
+    <field x="4"/>
+    <field x="8"/>
+    <field x="5"/>
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+      <x v="4"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="11"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="4"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x v="10"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="10"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x v="10"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x v="10"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x v="12"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="12"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x v="8"/>
+      <x v="1"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="12"/>
+      <x v="8"/>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+    <i>
+      <x v="13"/>
+      <x v="11"/>
+      <x v="2"/>
+      <x/>
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="10" hier="0"/>
+  </pageFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="KANBAN" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="A10:E20" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField name="Tipo" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
@@ -3020,9 +3232,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="KANBAN 2" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
-  <location ref="G10:K15" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="KANBAN 2" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+  <location ref="G10:K13" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField name="Tipo" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Item ID" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
@@ -3131,7 +3343,7 @@
     <field x="5"/>
     <field x="9"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="3">
     <i>
       <x v="10"/>
       <x v="4"/>
@@ -3147,223 +3359,11 @@
       <x/>
     </i>
     <i>
-      <x v="12"/>
-      <x v="8"/>
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i>
-      <x v="13"/>
-      <x v="11"/>
-      <x v="2"/>
-      <x/>
-      <x/>
-    </i>
-    <i>
       <x v="14"/>
       <x v="5"/>
       <x v="2"/>
       <x v="1"/>
       <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="10" hier="0"/>
-  </pageFields>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="KANBAN 3" cacheId="89" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
-  <location ref="M10:Q20" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="13">
-    <pivotField name="Tipo" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="Item ID" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="Tareas" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
-      <items count="39">
-        <item x="0"/>
-        <item x="9"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="23"/>
-        <item m="1" x="25"/>
-        <item x="22"/>
-        <item x="20"/>
-        <item m="1" x="35"/>
-        <item m="1" x="31"/>
-        <item m="1" x="28"/>
-        <item m="1" x="27"/>
-        <item m="1" x="30"/>
-        <item m="1" x="32"/>
-        <item m="1" x="38"/>
-        <item m="1" x="34"/>
-        <item m="1" x="37"/>
-        <item m="1" x="33"/>
-        <item m="1" x="26"/>
-        <item x="21"/>
-        <item x="24"/>
-        <item m="1" x="29"/>
-        <item m="1" x="36"/>
-      </items>
-    </pivotField>
-    <pivotField name="Predecesor" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="Responsable" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
-      <items count="14">
-        <item m="1" x="11"/>
-        <item m="1" x="13"/>
-        <item m="1" x="9"/>
-        <item m="1" x="7"/>
-        <item x="0"/>
-        <item x="5"/>
-        <item m="1" x="12"/>
-        <item m="1" x="8"/>
-        <item x="3"/>
-        <item m="1" x="10"/>
-        <item x="1"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="6"/>
-      </items>
-    </pivotField>
-    <pivotField name="Prioridad" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField name="Inicio" compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="Fin" compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="Vencimiento" axis="axisRow" compact="0" numFmtId="165" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
-      <items count="5">
-        <item m="1" x="4"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-      </items>
-    </pivotField>
-    <pivotField name="Situacion" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="3">
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField name="Estado" axis="axisPage" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField name="Progreso" compact="0" numFmtId="9" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="Trabajo_Hrs" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="5">
-    <field x="2"/>
-    <field x="4"/>
-    <field x="8"/>
-    <field x="5"/>
-    <field x="9"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-      <x v="4"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-      <x v="11"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="4"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x v="10"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="4"/>
-      <x v="10"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="5"/>
-      <x v="10"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="6"/>
-      <x v="10"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="7"/>
-      <x v="12"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="8"/>
-      <x v="12"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="9"/>
-      <x v="8"/>
-      <x v="1"/>
-      <x/>
-      <x v="1"/>
     </i>
   </rowItems>
   <colItems count="1">
@@ -3660,8 +3660,8 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="D11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3680,165 +3680,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
-      <c r="Q1" s="57"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="88"/>
     </row>
     <row r="2" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74"/>
       <c r="D2" s="1">
         <v>45013</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="72" t="s">
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="45"/>
-      <c r="L2" s="46"/>
-      <c r="N2" s="58" t="s">
+      <c r="K2" s="73"/>
+      <c r="L2" s="74"/>
+      <c r="N2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="59" t="s">
+      <c r="O2" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
     </row>
     <row r="3" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="72" t="s">
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="46"/>
-      <c r="N3" s="61" t="s">
+      <c r="K3" s="73"/>
+      <c r="L3" s="74"/>
+      <c r="N3" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="59" t="s">
+      <c r="O3" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
     </row>
     <row r="4" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="73" t="s">
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="46"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="66" t="s">
+      <c r="K4" s="73"/>
+      <c r="L4" s="74"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
     </row>
     <row r="5" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="46"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="49">
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75">
         <v>944198194</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="46"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="62" t="s">
+      <c r="K5" s="73"/>
+      <c r="L5" s="74"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="77"/>
     </row>
     <row r="6" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="46"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="74"/>
       <c r="D6" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="49">
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="75">
         <v>20600763246</v>
       </c>
-      <c r="K6" s="45"/>
-      <c r="L6" s="46"/>
-      <c r="N6" s="61"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="64"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="74"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="76"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="77"/>
     </row>
     <row r="7" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
@@ -3858,530 +3858,530 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="87" t="s">
+      <c r="D9" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="86" t="s">
+      <c r="E9" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="86" t="s">
+      <c r="F9" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="86" t="s">
+      <c r="H9" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="86" t="s">
+      <c r="I9" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="86" t="s">
+      <c r="J9" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="86" t="s">
+      <c r="K9" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="86" t="s">
+      <c r="L9" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="86" t="s">
+      <c r="M9" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="86" t="s">
+      <c r="N9" s="58" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="89">
+      <c r="C10" s="60">
         <v>1</v>
       </c>
-      <c r="D10" s="90" t="s">
+      <c r="D10" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="89">
+      <c r="E10" s="60">
         <v>1</v>
       </c>
-      <c r="F10" s="91" t="s">
+      <c r="F10" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="G10" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="92">
+      <c r="H10" s="62">
         <v>45024</v>
       </c>
-      <c r="I10" s="93">
+      <c r="I10" s="63">
         <v>45026</v>
       </c>
-      <c r="J10" s="94">
+      <c r="J10" s="64">
         <v>45027</v>
       </c>
-      <c r="K10" s="58" t="s">
+      <c r="K10" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="58" t="s">
+      <c r="L10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="95">
+      <c r="M10" s="65">
         <v>1</v>
       </c>
-      <c r="N10" s="58">
+      <c r="N10" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
-      <c r="B11" s="58" t="s">
+      <c r="A11" s="71"/>
+      <c r="B11" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="89">
+      <c r="C11" s="60">
         <v>2</v>
       </c>
-      <c r="D11" s="90" t="s">
+      <c r="D11" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="89">
+      <c r="E11" s="60">
         <v>1</v>
       </c>
-      <c r="F11" s="91" t="s">
+      <c r="F11" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="58" t="s">
+      <c r="G11" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="92">
+      <c r="H11" s="62">
         <v>45024</v>
       </c>
-      <c r="I11" s="93">
+      <c r="I11" s="63">
         <v>45026</v>
       </c>
-      <c r="J11" s="94">
+      <c r="J11" s="64">
         <v>45027</v>
       </c>
-      <c r="K11" s="58" t="s">
+      <c r="K11" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="58" t="s">
+      <c r="L11" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M11" s="95">
+      <c r="M11" s="65">
         <v>1</v>
       </c>
-      <c r="N11" s="58">
+      <c r="N11" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="88"/>
-      <c r="B12" s="58" t="s">
+      <c r="A12" s="71"/>
+      <c r="B12" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="89">
+      <c r="C12" s="60">
         <v>3</v>
       </c>
-      <c r="D12" s="90" t="s">
+      <c r="D12" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="89">
+      <c r="E12" s="60">
         <v>1</v>
       </c>
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="92">
+      <c r="H12" s="62">
         <v>45024</v>
       </c>
-      <c r="I12" s="93">
+      <c r="I12" s="63">
         <v>45026</v>
       </c>
-      <c r="J12" s="94">
+      <c r="J12" s="64">
         <v>45027</v>
       </c>
-      <c r="K12" s="58" t="s">
+      <c r="K12" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="58" t="s">
+      <c r="L12" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M12" s="95">
+      <c r="M12" s="65">
         <v>1</v>
       </c>
-      <c r="N12" s="58">
+      <c r="N12" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
-      <c r="B13" s="58" t="s">
+      <c r="A13" s="71"/>
+      <c r="B13" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="89">
+      <c r="C13" s="60">
         <v>4</v>
       </c>
-      <c r="D13" s="90" t="s">
+      <c r="D13" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="89">
+      <c r="E13" s="60">
         <v>1</v>
       </c>
-      <c r="F13" s="91" t="s">
+      <c r="F13" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="58" t="s">
+      <c r="G13" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="92">
+      <c r="H13" s="62">
         <v>45024</v>
       </c>
-      <c r="I13" s="93">
+      <c r="I13" s="63">
         <v>45026</v>
       </c>
-      <c r="J13" s="94">
+      <c r="J13" s="64">
         <v>45027</v>
       </c>
-      <c r="K13" s="58" t="s">
+      <c r="K13" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="58" t="s">
+      <c r="L13" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="95">
+      <c r="M13" s="65">
         <v>1</v>
       </c>
-      <c r="N13" s="58">
+      <c r="N13" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
-      <c r="B14" s="58" t="s">
+      <c r="A14" s="71"/>
+      <c r="B14" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="89">
+      <c r="C14" s="60">
         <v>5</v>
       </c>
-      <c r="D14" s="90" t="s">
+      <c r="D14" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="89">
+      <c r="E14" s="60">
         <v>1</v>
       </c>
-      <c r="F14" s="91" t="s">
+      <c r="F14" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="G14" s="58" t="s">
+      <c r="G14" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="92">
+      <c r="H14" s="62">
         <v>45024</v>
       </c>
-      <c r="I14" s="93">
+      <c r="I14" s="63">
         <v>45026</v>
       </c>
-      <c r="J14" s="94">
+      <c r="J14" s="64">
         <v>45027</v>
       </c>
-      <c r="K14" s="58" t="s">
+      <c r="K14" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="58" t="s">
+      <c r="L14" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M14" s="95">
+      <c r="M14" s="65">
         <v>1</v>
       </c>
-      <c r="N14" s="58">
+      <c r="N14" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="58" t="s">
+      <c r="A15" s="71"/>
+      <c r="B15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="89">
+      <c r="C15" s="60">
         <v>6</v>
       </c>
-      <c r="D15" s="90" t="s">
+      <c r="D15" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="89">
+      <c r="E15" s="60">
         <v>1</v>
       </c>
-      <c r="F15" s="91" t="s">
+      <c r="F15" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="58" t="s">
+      <c r="G15" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="62">
         <v>45024</v>
       </c>
-      <c r="I15" s="93">
+      <c r="I15" s="63">
         <v>45026</v>
       </c>
-      <c r="J15" s="94">
+      <c r="J15" s="64">
         <v>45027</v>
       </c>
-      <c r="K15" s="58" t="s">
+      <c r="K15" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="58" t="s">
+      <c r="L15" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="96">
+      <c r="M15" s="66">
         <v>1</v>
       </c>
-      <c r="N15" s="58">
+      <c r="N15" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
-      <c r="B16" s="58" t="s">
+      <c r="A16" s="71"/>
+      <c r="B16" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="89">
+      <c r="C16" s="60">
         <v>7</v>
       </c>
-      <c r="D16" s="97" t="s">
+      <c r="D16" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="89">
+      <c r="E16" s="60">
         <v>1</v>
       </c>
-      <c r="F16" s="91" t="s">
+      <c r="F16" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="58" t="s">
+      <c r="G16" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="92">
+      <c r="H16" s="62">
         <v>45024</v>
       </c>
-      <c r="I16" s="93">
+      <c r="I16" s="63">
         <v>45026</v>
       </c>
-      <c r="J16" s="94">
+      <c r="J16" s="64">
         <v>45027</v>
       </c>
-      <c r="K16" s="58" t="s">
+      <c r="K16" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="58" t="s">
+      <c r="L16" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M16" s="96">
+      <c r="M16" s="66">
         <v>1</v>
       </c>
-      <c r="N16" s="58">
+      <c r="N16" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
-      <c r="B17" s="58" t="s">
+      <c r="A17" s="71"/>
+      <c r="B17" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="89">
+      <c r="C17" s="60">
         <v>8</v>
       </c>
-      <c r="D17" s="97" t="s">
+      <c r="D17" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="89">
+      <c r="E17" s="60">
         <v>1</v>
       </c>
-      <c r="F17" s="91" t="s">
+      <c r="F17" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G17" s="58" t="s">
+      <c r="G17" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="92">
+      <c r="H17" s="62">
         <v>45024</v>
       </c>
-      <c r="I17" s="93">
+      <c r="I17" s="63">
         <v>45026</v>
       </c>
-      <c r="J17" s="94">
+      <c r="J17" s="64">
         <v>45027</v>
       </c>
-      <c r="K17" s="58" t="s">
+      <c r="K17" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="58" t="s">
+      <c r="L17" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M17" s="96">
+      <c r="M17" s="66">
         <v>1</v>
       </c>
-      <c r="N17" s="58">
+      <c r="N17" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
-      <c r="B18" s="58" t="s">
+      <c r="A18" s="71"/>
+      <c r="B18" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="89">
+      <c r="C18" s="60">
         <v>9</v>
       </c>
-      <c r="D18" s="98" t="s">
+      <c r="D18" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="89">
+      <c r="E18" s="60">
         <v>1</v>
       </c>
-      <c r="F18" s="91" t="s">
+      <c r="F18" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="58" t="s">
+      <c r="G18" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="92">
+      <c r="H18" s="62">
         <v>45024</v>
       </c>
-      <c r="I18" s="93">
+      <c r="I18" s="63">
         <v>45026</v>
       </c>
-      <c r="J18" s="94">
+      <c r="J18" s="64">
         <v>45027</v>
       </c>
-      <c r="K18" s="58" t="s">
+      <c r="K18" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L18" s="58" t="s">
+      <c r="L18" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="96">
+      <c r="M18" s="66">
         <v>1</v>
       </c>
-      <c r="N18" s="58">
+      <c r="N18" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
-      <c r="B19" s="58" t="s">
+      <c r="A19" s="71"/>
+      <c r="B19" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="89">
+      <c r="C19" s="60">
         <v>10</v>
       </c>
-      <c r="D19" s="97" t="s">
+      <c r="D19" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="89">
+      <c r="E19" s="60">
         <v>1</v>
       </c>
-      <c r="F19" s="91" t="s">
+      <c r="F19" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="92">
+      <c r="H19" s="62">
         <v>45024</v>
       </c>
-      <c r="I19" s="93">
+      <c r="I19" s="63">
         <v>45026</v>
       </c>
-      <c r="J19" s="94">
+      <c r="J19" s="64">
         <v>45027</v>
       </c>
-      <c r="K19" s="58" t="s">
+      <c r="K19" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="L19" s="58" t="s">
+      <c r="L19" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="96">
+      <c r="M19" s="66">
         <v>1</v>
       </c>
-      <c r="N19" s="58">
+      <c r="N19" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="80">
+      <c r="C20" s="52">
         <v>8</v>
       </c>
-      <c r="D20" s="81" t="s">
+      <c r="D20" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="80">
+      <c r="E20" s="52">
         <v>1</v>
       </c>
-      <c r="F20" s="82" t="s">
+      <c r="F20" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="G20" s="79" t="s">
+      <c r="G20" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="H20" s="83">
+      <c r="H20" s="55">
         <v>45028</v>
       </c>
-      <c r="I20" s="84">
+      <c r="I20" s="56">
         <v>45054</v>
       </c>
-      <c r="J20" s="85">
+      <c r="J20" s="57">
         <v>45055</v>
       </c>
-      <c r="K20" s="79" t="s">
+      <c r="K20" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="79" t="s">
+      <c r="L20" s="51" t="s">
         <v>42</v>
       </c>
       <c r="M20" s="13">
         <v>0</v>
       </c>
-      <c r="N20" s="79">
+      <c r="N20" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="67"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="8">
         <v>9</v>
       </c>
-      <c r="D21" s="74" t="s">
+      <c r="D21" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="76" t="s">
+      <c r="E21" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="71" t="s">
+      <c r="F21" s="46" t="s">
         <v>75</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -4390,7 +4390,7 @@
       <c r="H21" s="9">
         <v>45028</v>
       </c>
-      <c r="I21" s="75">
+      <c r="I21" s="48">
         <v>45054</v>
       </c>
       <c r="J21" s="11">
@@ -4403,27 +4403,27 @@
         <v>42</v>
       </c>
       <c r="M21" s="13">
-        <v>0</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="N21" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="67"/>
+      <c r="A22" s="83"/>
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C22" s="8">
         <v>10</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="47" t="s">
         <v>85</v>
       </c>
       <c r="E22" s="8">
         <v>8</v>
       </c>
-      <c r="F22" s="71" t="s">
+      <c r="F22" s="46" t="s">
         <v>78</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -4432,8 +4432,8 @@
       <c r="H22" s="9">
         <v>45028</v>
       </c>
-      <c r="I22" s="75">
-        <v>45053</v>
+      <c r="I22" s="9">
+        <v>45028</v>
       </c>
       <c r="J22" s="11">
         <v>45055</v>
@@ -4442,30 +4442,30 @@
         <v>41</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="M22" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="67"/>
+      <c r="A23" s="83"/>
       <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="8">
         <v>11</v>
       </c>
-      <c r="D23" s="74" t="s">
+      <c r="D23" s="47" t="s">
         <v>86</v>
       </c>
       <c r="E23" s="14">
         <v>10</v>
       </c>
-      <c r="F23" s="71" t="s">
+      <c r="F23" s="46" t="s">
         <v>79</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -4474,8 +4474,8 @@
       <c r="H23" s="9">
         <v>45028</v>
       </c>
-      <c r="I23" s="75">
-        <v>45053</v>
+      <c r="I23" s="9">
+        <v>45028</v>
       </c>
       <c r="J23" s="11">
         <v>45055</v>
@@ -4484,39 +4484,39 @@
         <v>41</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="M23" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="67"/>
+      <c r="A24" s="83"/>
       <c r="B24" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="8">
         <v>12</v>
       </c>
-      <c r="D24" s="74" t="s">
+      <c r="D24" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="E24" s="77" t="s">
+      <c r="E24" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="F24" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="G24" s="71" t="s">
+      <c r="G24" s="46" t="s">
         <v>44</v>
       </c>
       <c r="H24" s="9">
         <v>45028</v>
       </c>
-      <c r="I24" s="75">
+      <c r="I24" s="48">
         <v>45054</v>
       </c>
       <c r="J24" s="11">
@@ -4536,7 +4536,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="69" t="s">
+      <c r="A25" s="82" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -4545,7 +4545,7 @@
       <c r="C25" s="8">
         <v>14</v>
       </c>
-      <c r="D25" s="99" t="s">
+      <c r="D25" s="69" t="s">
         <v>91</v>
       </c>
       <c r="E25" s="8"/>
@@ -4570,14 +4570,14 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="67"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="8">
         <v>15</v>
       </c>
-      <c r="D26" s="99" t="s">
+      <c r="D26" s="69" t="s">
         <v>92</v>
       </c>
       <c r="E26" s="8"/>
@@ -4602,14 +4602,14 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="67"/>
+      <c r="A27" s="83"/>
       <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C27" s="8">
         <v>16</v>
       </c>
-      <c r="D27" s="99" t="s">
+      <c r="D27" s="69" t="s">
         <v>93</v>
       </c>
       <c r="E27" s="8"/>
@@ -4634,14 +4634,14 @@
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="67"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="8">
         <v>17</v>
       </c>
-      <c r="D28" s="99" t="s">
+      <c r="D28" s="69" t="s">
         <v>94</v>
       </c>
       <c r="E28" s="8"/>
@@ -4666,14 +4666,14 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
+      <c r="A29" s="84"/>
       <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="8">
         <v>18</v>
       </c>
-      <c r="D29" s="99" t="s">
+      <c r="D29" s="69" t="s">
         <v>95</v>
       </c>
       <c r="E29" s="8"/>
@@ -4698,7 +4698,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="85" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -4707,7 +4707,7 @@
       <c r="C30" s="8">
         <v>19</v>
       </c>
-      <c r="D30" s="100" t="s">
+      <c r="D30" s="70" t="s">
         <v>47</v>
       </c>
       <c r="E30" s="8"/>
@@ -4732,14 +4732,14 @@
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="67"/>
+      <c r="A31" s="83"/>
       <c r="B31" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="8">
         <v>20</v>
       </c>
-      <c r="D31" s="100" t="s">
+      <c r="D31" s="70" t="s">
         <v>48</v>
       </c>
       <c r="E31" s="8"/>
@@ -4764,14 +4764,14 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="67"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="8">
         <v>21</v>
       </c>
-      <c r="D32" s="100" t="s">
+      <c r="D32" s="70" t="s">
         <v>96</v>
       </c>
       <c r="E32" s="8"/>
@@ -4796,14 +4796,14 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="67"/>
+      <c r="A33" s="83"/>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="8">
         <v>22</v>
       </c>
-      <c r="D33" s="100" t="s">
+      <c r="D33" s="70" t="s">
         <v>97</v>
       </c>
       <c r="E33" s="8"/>
@@ -4828,14 +4828,14 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="68"/>
+      <c r="A34" s="84"/>
       <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="8">
         <v>23</v>
       </c>
-      <c r="D34" s="100" t="s">
+      <c r="D34" s="70" t="s">
         <v>98</v>
       </c>
       <c r="E34" s="8"/>
@@ -4965,16 +4965,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="N3:N6"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="A30:A34"/>
@@ -4991,6 +4981,16 @@
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F4:I4"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="O6:Q6"/>
+    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <conditionalFormatting sqref="M10:M41">
     <cfRule type="colorScale" priority="17">
@@ -5053,7 +5053,7 @@
   <dimension ref="B27:J52"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5062,7 +5062,7 @@
     <col min="8" max="8" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="28" t="s">
         <v>15</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="30" t="s">
         <v>40</v>
       </c>
@@ -5117,10 +5117,10 @@
         <v>1</v>
       </c>
       <c r="J28" s="39">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+        <v>8.1083272520878935E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="40"/>
       <c r="C29" s="30" t="s">
         <v>74</v>
@@ -5144,10 +5144,10 @@
         <v>1</v>
       </c>
       <c r="J29" s="39">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+        <v>8.1083272520878935E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="40"/>
       <c r="C30" s="30" t="s">
         <v>83</v>
@@ -5168,13 +5168,13 @@
         <v>42</v>
       </c>
       <c r="I30" s="38">
-        <v>0</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="J30" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+        <v>2.7000729749452688E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="40"/>
       <c r="C31" s="30" t="s">
         <v>87</v>
@@ -5201,7 +5201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="40"/>
       <c r="C32" s="30" t="s">
         <v>91</v>
@@ -5226,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="40"/>
       <c r="C33" s="30" t="s">
         <v>92</v>
@@ -5251,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="40"/>
       <c r="C34" s="30" t="s">
         <v>93</v>
@@ -5276,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="40"/>
       <c r="C35" s="30" t="s">
         <v>94</v>
@@ -5301,7 +5301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="40"/>
       <c r="C36" s="30" t="s">
         <v>95</v>
@@ -5326,7 +5326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="40"/>
       <c r="C37" s="30" t="s">
         <v>97</v>
@@ -5351,7 +5351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="40"/>
       <c r="C38" s="30" t="s">
         <v>96</v>
@@ -5376,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="40"/>
       <c r="C39" s="30" t="s">
         <v>47</v>
@@ -5401,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="40"/>
       <c r="C40" s="30" t="s">
         <v>48</v>
@@ -5426,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B41" s="40"/>
       <c r="C41" s="30" t="s">
         <v>98</v>
@@ -5451,7 +5451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B42" s="30" t="s">
         <v>29</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>1</v>
       </c>
       <c r="J42" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5504,7 +5504,7 @@
         <v>1</v>
       </c>
       <c r="J43" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5531,7 +5531,7 @@
         <v>1</v>
       </c>
       <c r="J44" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="45" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5558,7 +5558,7 @@
         <v>1</v>
       </c>
       <c r="J45" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5585,7 +5585,7 @@
         <v>1</v>
       </c>
       <c r="J46" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5639,7 +5639,7 @@
         <v>1</v>
       </c>
       <c r="J48" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5666,7 +5666,7 @@
         <v>1</v>
       </c>
       <c r="J49" s="39">
-        <v>0.1</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5714,13 +5714,13 @@
         <v>41</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I51" s="38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" s="39">
-        <v>0</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5741,13 +5741,13 @@
         <v>41</v>
       </c>
       <c r="H52" s="33" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I52" s="42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" s="43">
-        <v>0</v>
+        <v>8.1083272520878935E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5762,8 +5762,8 @@
   </sheetPr>
   <dimension ref="A1:AB1007"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5870,46 +5870,46 @@
       <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="52"/>
-      <c r="G6" s="50" t="s">
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="95"/>
+      <c r="G6" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-      <c r="K6" s="52"/>
-      <c r="M6" s="50" t="s">
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="95"/>
+      <c r="M6" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="N6" s="51"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="95"/>
     </row>
     <row r="7" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="55"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="55"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="98"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="55"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="98"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
@@ -6110,19 +6110,19 @@
       <c r="E13" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="I13" s="31">
+      <c r="G13" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" s="34">
         <v>45055</v>
       </c>
-      <c r="J13" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="37" t="s">
+      <c r="J13" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="36" t="s">
         <v>41</v>
       </c>
       <c r="M13" s="30" t="s">
@@ -6157,21 +6157,6 @@
       <c r="E14" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="31">
-        <v>45055</v>
-      </c>
-      <c r="J14" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="K14" s="37" t="s">
-        <v>41</v>
-      </c>
       <c r="M14" s="30" t="s">
         <v>35</v>
       </c>
@@ -6202,21 +6187,6 @@
         <v>63</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="I15" s="34">
-        <v>45055</v>
-      </c>
-      <c r="J15" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15" s="36" t="s">
         <v>41</v>
       </c>
       <c r="M15" s="30" t="s">
@@ -6399,23 +6369,23 @@
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="25"/>
-      <c r="M20" s="33" t="s">
+      <c r="M20" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="N20" s="33" t="s">
+      <c r="N20" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="O20" s="34">
+      <c r="O20" s="31">
         <v>45027</v>
       </c>
-      <c r="P20" s="33" t="s">
+      <c r="P20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="Q20" s="36" t="s">
+      <c r="Q20" s="37" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -6426,13 +6396,23 @@
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="25"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="25"/>
-    </row>
-    <row r="22" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M21" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="N21" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="O21" s="31">
+        <v>45055</v>
+      </c>
+      <c r="P21" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -6443,11 +6423,21 @@
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="25"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="25"/>
+      <c r="M22" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="N22" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="O22" s="34">
+        <v>45055</v>
+      </c>
+      <c r="P22" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q22" s="36" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
@@ -23279,8 +23269,8 @@
   </sheetPr>
   <dimension ref="B1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
actualizado parte mauricio y eduardo - entregable 2
</commit_message>
<xml_diff>
--- a/G3-Tablero Kanban_ Calidad y Mejora Continua.xlsx
+++ b/G3-Tablero Kanban_ Calidad y Mejora Continua.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\TECSUP\AÑO 2 - SEMESTRE 3\MejContinua\Kanban\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauri\Downloads\dashboardMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE384D75-C02B-442F-AD0E-E40A465B4DB6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2032F701-20C9-45CF-B0E2-6AF8FA2DB5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,8 +29,8 @@
     <customWorkbookView name="Filtro 1" guid="{6D37D4BD-4770-4892-8DF3-C2DF475ACC4D}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <pivotCaches>
-    <pivotCache cacheId="29" r:id="rId5"/>
-    <pivotCache cacheId="37" r:id="rId6"/>
+    <pivotCache cacheId="9" r:id="rId5"/>
+    <pivotCache cacheId="19" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -362,7 +362,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -469,6 +469,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="17">
@@ -873,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -995,18 +1003,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1025,14 +1021,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1041,6 +1049,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1419,7 +1428,133 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HP" refreshedDate="45053.872638310182" refreshedVersion="6" recordCount="26" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Mauricio E." refreshedDate="45054.569391666664" refreshedVersion="8" recordCount="25" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B9:N34" sheet="DATOS"/>
+  </cacheSource>
+  <cacheFields count="13">
+    <cacheField name="Tipo" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Item ID" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="23"/>
+    </cacheField>
+    <cacheField name="Tareas" numFmtId="0">
+      <sharedItems count="39">
+        <s v="1.1.1.Breve descripción de la empresa y reseña histórica"/>
+        <s v="1.1.2.Organigrama"/>
+        <s v="1.1.3.Descripción de los productos o servicios ofrecidos"/>
+        <s v="1.1.4.Visión"/>
+        <s v="1.1.5.Misión"/>
+        <s v="1.1.6.Valores empresariales"/>
+        <s v="1.1.7.Definicion del Problema"/>
+        <s v="1.1.8.Objetivos"/>
+        <s v="1.1.9.Diagrama de bloques de productos o servicios ofrecidos por la empresa"/>
+        <s v="1.1.10.Mapa de procesos"/>
+        <s v="2.1. Lluvia de ideas"/>
+        <s v="2.2.Diagramas de Afinidad"/>
+        <s v="2.3. Tecnica de los porques"/>
+        <s v="2.4. Diagrama de Ishikawa"/>
+        <s v="2.5. Diagrama de Pareto"/>
+        <s v="3.1. Arbol de soluciones"/>
+        <s v="3.2. Solucion a desperdicios detectados según Lean"/>
+        <s v="3.3. Metodologia 5&quot;s&quot;"/>
+        <s v="3.4. Metodologia 5W-2H"/>
+        <s v="3.5. Presupuesto"/>
+        <s v="Conclusiones"/>
+        <s v="Recomendaciones"/>
+        <s v="Bibliografía"/>
+        <s v="Anexos"/>
+        <s v="Resumen"/>
+        <s v="Árbol de soluciones" u="1"/>
+        <s v="Presupuesto" u="1"/>
+        <s v="Diagramas de Afinidad" u="1"/>
+        <s v="Diagrama de Pareto" u="1"/>
+        <s v="Solución a desperdicios detectados según Lean" u="1"/>
+        <s v="Lluvia de ideas" u="1"/>
+        <s v="Diagrama de Ishikawa" u="1"/>
+        <s v="Mapa de procesos" u="1"/>
+        <s v="Objetivos general" u="1"/>
+        <s v="Metodología 5W-2H" u="1"/>
+        <s v="Diagrama de bloques de productos o servicios ofrecidos por la empresa" u="1"/>
+        <s v="Técnica del Porqués" u="1"/>
+        <s v="Objetivos específicos" u="1"/>
+        <s v="Metodología 5S" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Predecesor" numFmtId="0">
+      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
+    </cacheField>
+    <cacheField name="Responsable" numFmtId="0">
+      <sharedItems containsBlank="1" count="14">
+        <s v="Eduardo"/>
+        <s v="Mauricio"/>
+        <s v="Todos"/>
+        <s v="Juan"/>
+        <s v="Neals"/>
+        <s v="Eduardo/Mauricio"/>
+        <m/>
+        <s v="Edu" u="1"/>
+        <s v="Franshesco" u="1"/>
+        <s v="Diegooooo" u="1"/>
+        <s v="Krisbel" u="1"/>
+        <s v="Angel" u="1"/>
+        <s v="Fernando" u="1"/>
+        <s v="Diego " u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Prioridad" numFmtId="0">
+      <sharedItems containsBlank="1" count="3">
+        <s v="Alta"/>
+        <s v="Media"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Inicio" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-04-08T00:00:00" maxDate="2023-06-08T00:00:00"/>
+    </cacheField>
+    <cacheField name="Fin" numFmtId="165">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-04-10T00:00:00" maxDate="2023-05-09T00:00:00"/>
+    </cacheField>
+    <cacheField name="Vencimiento" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-04-10T00:00:00" maxDate="2023-07-05T00:00:00" count="5">
+        <d v="2023-04-11T00:00:00"/>
+        <d v="2023-05-09T00:00:00"/>
+        <d v="2023-06-06T00:00:00"/>
+        <d v="2023-07-04T00:00:00"/>
+        <d v="2023-04-10T00:00:00" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Situacion" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Vencido"/>
+        <s v="En plazo"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Estado" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Hecho"/>
+        <s v="Haciendo"/>
+        <s v="Por hacer"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Progreso" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Trabajo_Hrs" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="2"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Mauricio E." refreshedDate="45054.569392129626" refreshedVersion="8" recordCount="26" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B9:N35" sheet="DATOS"/>
   </cacheSource>
@@ -1557,133 +1692,387 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HP" refreshedDate="45053.872885879631" refreshedVersion="6" recordCount="25" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="B9:N34" sheet="DATOS"/>
-  </cacheSource>
-  <cacheFields count="13">
-    <cacheField name="Tipo" numFmtId="0">
-      <sharedItems/>
-    </cacheField>
-    <cacheField name="Item ID" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="23"/>
-    </cacheField>
-    <cacheField name="Tareas" numFmtId="0">
-      <sharedItems count="39">
-        <s v="1.1.1.Breve descripción de la empresa y reseña histórica"/>
-        <s v="1.1.2.Organigrama"/>
-        <s v="1.1.3.Descripción de los productos o servicios ofrecidos"/>
-        <s v="1.1.4.Visión"/>
-        <s v="1.1.5.Misión"/>
-        <s v="1.1.6.Valores empresariales"/>
-        <s v="1.1.7.Definicion del Problema"/>
-        <s v="1.1.8.Objetivos"/>
-        <s v="1.1.9.Diagrama de bloques de productos o servicios ofrecidos por la empresa"/>
-        <s v="1.1.10.Mapa de procesos"/>
-        <s v="2.1. Lluvia de ideas"/>
-        <s v="2.2.Diagramas de Afinidad"/>
-        <s v="2.3. Tecnica de los porques"/>
-        <s v="2.4. Diagrama de Ishikawa"/>
-        <s v="2.5. Diagrama de Pareto"/>
-        <s v="3.1. Arbol de soluciones"/>
-        <s v="3.2. Solucion a desperdicios detectados según Lean"/>
-        <s v="3.3. Metodologia 5&quot;s&quot;"/>
-        <s v="3.4. Metodologia 5W-2H"/>
-        <s v="3.5. Presupuesto"/>
-        <s v="Conclusiones"/>
-        <s v="Recomendaciones"/>
-        <s v="Bibliografía"/>
-        <s v="Anexos"/>
-        <s v="Resumen"/>
-        <s v="Árbol de soluciones" u="1"/>
-        <s v="Presupuesto" u="1"/>
-        <s v="Diagramas de Afinidad" u="1"/>
-        <s v="Diagrama de Pareto" u="1"/>
-        <s v="Solución a desperdicios detectados según Lean" u="1"/>
-        <s v="Lluvia de ideas" u="1"/>
-        <s v="Diagrama de Ishikawa" u="1"/>
-        <s v="Mapa de procesos" u="1"/>
-        <s v="Objetivos general" u="1"/>
-        <s v="Metodología 5W-2H" u="1"/>
-        <s v="Diagrama de bloques de productos o servicios ofrecidos por la empresa" u="1"/>
-        <s v="Técnica del Porqués" u="1"/>
-        <s v="Objetivos específicos" u="1"/>
-        <s v="Metodología 5S" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Predecesor" numFmtId="0">
-      <sharedItems containsBlank="1" containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="10"/>
-    </cacheField>
-    <cacheField name="Responsable" numFmtId="0">
-      <sharedItems containsBlank="1" count="14">
-        <s v="Eduardo"/>
-        <s v="Mauricio"/>
-        <s v="Todos"/>
-        <s v="Juan"/>
-        <s v="Neals"/>
-        <s v="Eduardo/Mauricio"/>
-        <m/>
-        <s v="Edu" u="1"/>
-        <s v="Franshesco" u="1"/>
-        <s v="Diegooooo" u="1"/>
-        <s v="Krisbel" u="1"/>
-        <s v="Angel" u="1"/>
-        <s v="Fernando" u="1"/>
-        <s v="Diego " u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Prioridad" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
-        <s v="Alta"/>
-        <s v="Media"/>
-        <m/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Inicio" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-04-08T00:00:00" maxDate="2023-06-08T00:00:00"/>
-    </cacheField>
-    <cacheField name="Fin" numFmtId="165">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-04-10T00:00:00" maxDate="2023-05-09T00:00:00"/>
-    </cacheField>
-    <cacheField name="Vencimiento" numFmtId="165">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2023-04-10T00:00:00" maxDate="2023-07-05T00:00:00" count="5">
-        <d v="2023-04-11T00:00:00"/>
-        <d v="2023-05-09T00:00:00"/>
-        <d v="2023-06-06T00:00:00"/>
-        <d v="2023-07-04T00:00:00"/>
-        <d v="2023-04-10T00:00:00" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Situacion" numFmtId="0">
-      <sharedItems count="2">
-        <s v="Vencido"/>
-        <s v="En plazo"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Estado" numFmtId="0">
-      <sharedItems count="3">
-        <s v="Hecho"/>
-        <s v="Haciendo"/>
-        <s v="Por hacer"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Progreso" numFmtId="9">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="1"/>
-    </cacheField>
-    <cacheField name="Trabajo_Hrs" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="2"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="25">
+  <r>
+    <s v="Personal"/>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="2"/>
+    <x v="1"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="3"/>
+    <x v="2"/>
+    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="4"/>
+    <x v="3"/>
+    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="5"/>
+    <x v="4"/>
+    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="6"/>
+    <x v="5"/>
+    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="7"/>
+    <x v="6"/>
+    <n v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="8"/>
+    <x v="7"/>
+    <n v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="9"/>
+    <x v="8"/>
+    <n v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="10"/>
+    <x v="9"/>
+    <n v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <d v="2023-04-08T00:00:00"/>
+    <d v="2023-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="8"/>
+    <x v="10"/>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <d v="2023-04-12T00:00:00"/>
+    <d v="2023-05-08T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="9"/>
+    <x v="11"/>
+    <s v="9,10"/>
+    <x v="2"/>
+    <x v="0"/>
+    <d v="2023-04-12T00:00:00"/>
+    <d v="2023-05-08T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0.33300000000000002"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="10"/>
+    <x v="12"/>
+    <n v="8"/>
+    <x v="3"/>
+    <x v="0"/>
+    <d v="2023-04-12T00:00:00"/>
+    <d v="2023-04-12T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Personal"/>
+    <n v="11"/>
+    <x v="13"/>
+    <n v="10"/>
+    <x v="4"/>
+    <x v="0"/>
+    <d v="2023-04-12T00:00:00"/>
+    <d v="2023-04-12T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="12"/>
+    <x v="14"/>
+    <s v="8,9,10,11,12"/>
+    <x v="5"/>
+    <x v="1"/>
+    <d v="2023-04-12T00:00:00"/>
+    <d v="2023-05-08T00:00:00"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="14"/>
+    <x v="15"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-04-10T00:00:00"/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="15"/>
+    <x v="16"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-04-10T00:00:00"/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="16"/>
+    <x v="17"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-04-10T00:00:00"/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="17"/>
+    <x v="18"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-04-10T00:00:00"/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="18"/>
+    <x v="19"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-04-10T00:00:00"/>
+    <m/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="19"/>
+    <x v="20"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-06-07T00:00:00"/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="20"/>
+    <x v="21"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-06-07T00:00:00"/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="21"/>
+    <x v="22"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-06-07T00:00:00"/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="22"/>
+    <x v="23"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-06-07T00:00:00"/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Equipo"/>
+    <n v="23"/>
+    <x v="24"/>
+    <m/>
+    <x v="6"/>
+    <x v="2"/>
+    <d v="2023-06-07T00:00:00"/>
+    <m/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="0"/>
+    <m/>
+  </r>
+</pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="26">
   <r>
     <x v="0"/>
@@ -2078,388 +2467,8 @@
 </pivotCacheRecords>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="25">
-  <r>
-    <s v="Personal"/>
-    <n v="1"/>
-    <x v="0"/>
-    <n v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="2"/>
-    <x v="1"/>
-    <n v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="3"/>
-    <x v="2"/>
-    <n v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="4"/>
-    <x v="3"/>
-    <n v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="5"/>
-    <x v="4"/>
-    <n v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="6"/>
-    <x v="5"/>
-    <n v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="7"/>
-    <x v="6"/>
-    <n v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="8"/>
-    <x v="7"/>
-    <n v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="9"/>
-    <x v="8"/>
-    <n v="1"/>
-    <x v="3"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="10"/>
-    <x v="9"/>
-    <n v="1"/>
-    <x v="4"/>
-    <x v="0"/>
-    <d v="2023-04-08T00:00:00"/>
-    <d v="2023-04-10T00:00:00"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="8"/>
-    <x v="10"/>
-    <n v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <d v="2023-04-12T00:00:00"/>
-    <d v="2023-05-08T00:00:00"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="9"/>
-    <x v="11"/>
-    <s v="9,10"/>
-    <x v="2"/>
-    <x v="0"/>
-    <d v="2023-04-12T00:00:00"/>
-    <d v="2023-05-08T00:00:00"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0.33300000000000002"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="10"/>
-    <x v="12"/>
-    <n v="8"/>
-    <x v="3"/>
-    <x v="0"/>
-    <d v="2023-04-12T00:00:00"/>
-    <d v="2023-04-12T00:00:00"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Personal"/>
-    <n v="11"/>
-    <x v="13"/>
-    <n v="10"/>
-    <x v="4"/>
-    <x v="0"/>
-    <d v="2023-04-12T00:00:00"/>
-    <d v="2023-04-12T00:00:00"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="1"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="12"/>
-    <x v="14"/>
-    <s v="8,9,10,11,12"/>
-    <x v="5"/>
-    <x v="1"/>
-    <d v="2023-04-12T00:00:00"/>
-    <d v="2023-05-08T00:00:00"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="0"/>
-    <n v="2"/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="14"/>
-    <x v="15"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-04-10T00:00:00"/>
-    <m/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="15"/>
-    <x v="16"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-04-10T00:00:00"/>
-    <m/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="16"/>
-    <x v="17"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-04-10T00:00:00"/>
-    <m/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="17"/>
-    <x v="18"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-04-10T00:00:00"/>
-    <m/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="18"/>
-    <x v="19"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-04-10T00:00:00"/>
-    <m/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="19"/>
-    <x v="20"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-06-07T00:00:00"/>
-    <m/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="20"/>
-    <x v="21"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-06-07T00:00:00"/>
-    <m/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="21"/>
-    <x v="22"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-06-07T00:00:00"/>
-    <m/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="22"/>
-    <x v="23"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-06-07T00:00:00"/>
-    <m/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-  <r>
-    <s v="Equipo"/>
-    <n v="23"/>
-    <x v="24"/>
-    <m/>
-    <x v="6"/>
-    <x v="2"/>
-    <d v="2023-06-07T00:00:00"/>
-    <m/>
-    <x v="3"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="0"/>
-    <m/>
-  </r>
-</pivotCacheRecords>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="DASHBOARD" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="DASHBOARD" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="B27:J52" firstHeaderRow="1" firstDataRow="1" firstDataCol="8"/>
   <pivotFields count="13">
     <pivotField name="Tipo" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending" defaultSubtotal="0">
@@ -2823,7 +2832,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="KANBAN 3" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000002000000}" name="KANBAN 3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="M10:Q22" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField name="Tipo" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
@@ -3035,7 +3044,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="KANBAN" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="KANBAN" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="A10:E20" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField name="Tipo" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
@@ -3233,7 +3242,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="KANBAN 2" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="6" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="KANBAN 2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="G10:K13" firstHeaderRow="1" firstDataRow="1" firstDataCol="5" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField name="Tipo" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
@@ -3660,8 +3669,8 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="D11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="D13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3680,165 +3689,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="79"/>
     </row>
     <row r="2" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="1">
         <v>45013</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="72" t="s">
+      <c r="F2" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="90" t="s">
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="73"/>
-      <c r="L2" s="74"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="81"/>
       <c r="N2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="76" t="s">
+      <c r="O2" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="77"/>
+      <c r="P2" s="87"/>
+      <c r="Q2" s="87"/>
     </row>
     <row r="3" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="74"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="74"/>
-      <c r="J3" s="90" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="73"/>
-      <c r="L3" s="74"/>
-      <c r="N3" s="81" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="81"/>
+      <c r="N3" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="76" t="s">
+      <c r="O3" s="86" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
     </row>
     <row r="4" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="81"/>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="72" t="s">
+      <c r="F4" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="91" t="s">
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="73"/>
-      <c r="L4" s="74"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="78" t="s">
+      <c r="K4" s="77"/>
+      <c r="L4" s="81"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
     </row>
     <row r="5" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="74"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="81"/>
       <c r="D5" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="75">
+      <c r="G5" s="77"/>
+      <c r="H5" s="77"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="92">
         <v>944198194</v>
       </c>
-      <c r="K5" s="73"/>
-      <c r="L5" s="74"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="80" t="s">
+      <c r="K5" s="77"/>
+      <c r="L5" s="81"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="77"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
     </row>
     <row r="6" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="74"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="81"/>
       <c r="D6" s="4" t="s">
         <v>66</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="72" t="s">
+      <c r="F6" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="75">
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="92">
         <v>20600763246</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="74"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="81"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
     </row>
     <row r="7" spans="1:17" ht="13.2" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
@@ -3902,7 +3911,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="91" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="44" t="s">
@@ -3946,7 +3955,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
+      <c r="A11" s="91"/>
       <c r="B11" s="44" t="s">
         <v>29</v>
       </c>
@@ -3988,7 +3997,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
+      <c r="A12" s="91"/>
       <c r="B12" s="44" t="s">
         <v>29</v>
       </c>
@@ -4030,7 +4039,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
+      <c r="A13" s="91"/>
       <c r="B13" s="44" t="s">
         <v>29</v>
       </c>
@@ -4072,7 +4081,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
+      <c r="A14" s="91"/>
       <c r="B14" s="44" t="s">
         <v>29</v>
       </c>
@@ -4114,7 +4123,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
+      <c r="A15" s="91"/>
       <c r="B15" s="44" t="s">
         <v>29</v>
       </c>
@@ -4156,7 +4165,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
+      <c r="A16" s="91"/>
       <c r="B16" s="44" t="s">
         <v>40</v>
       </c>
@@ -4198,7 +4207,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="71"/>
+      <c r="A17" s="91"/>
       <c r="B17" s="44" t="s">
         <v>40</v>
       </c>
@@ -4240,7 +4249,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="71"/>
+      <c r="A18" s="91"/>
       <c r="B18" s="44" t="s">
         <v>29</v>
       </c>
@@ -4282,7 +4291,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
+      <c r="A19" s="91"/>
       <c r="B19" s="44" t="s">
         <v>29</v>
       </c>
@@ -4324,7 +4333,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="85" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="51" t="s">
@@ -4361,14 +4370,14 @@
         <v>42</v>
       </c>
       <c r="M20" s="13">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="N20" s="51">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="83"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
@@ -4410,7 +4419,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
@@ -4452,7 +4461,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
@@ -4494,7 +4503,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
+      <c r="A24" s="73"/>
       <c r="B24" s="3" t="s">
         <v>40</v>
       </c>
@@ -4526,17 +4535,17 @@
         <v>41</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="M24" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="82" t="s">
+      <c r="A25" s="72" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -4570,7 +4579,7 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
+      <c r="A26" s="73"/>
       <c r="B26" s="3" t="s">
         <v>40</v>
       </c>
@@ -4602,7 +4611,7 @@
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="83"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="3" t="s">
         <v>40</v>
       </c>
@@ -4634,7 +4643,7 @@
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="83"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
@@ -4666,7 +4675,7 @@
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="84"/>
+      <c r="A29" s="74"/>
       <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
@@ -4698,7 +4707,7 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="75" t="s">
         <v>46</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -4732,7 +4741,7 @@
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
+      <c r="A31" s="73"/>
       <c r="B31" s="3" t="s">
         <v>40</v>
       </c>
@@ -4764,7 +4773,7 @@
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="83"/>
+      <c r="A32" s="73"/>
       <c r="B32" s="3" t="s">
         <v>40</v>
       </c>
@@ -4796,7 +4805,7 @@
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="83"/>
+      <c r="A33" s="73"/>
       <c r="B33" s="3" t="s">
         <v>40</v>
       </c>
@@ -4828,7 +4837,7 @@
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="84"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
@@ -4961,10 +4970,20 @@
   <customSheetViews>
     <customSheetView guid="{6D37D4BD-4770-4892-8DF3-C2DF475ACC4D}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="B9:N38" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
+      <autoFilter ref="B9:N38" xr:uid="{06DAF04F-481D-422A-932D-FDB512039E4F}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="26">
+    <mergeCell ref="A10:A19"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:Q4"/>
+    <mergeCell ref="O5:Q5"/>
+    <mergeCell ref="O6:Q6"/>
     <mergeCell ref="N3:N6"/>
     <mergeCell ref="A25:A29"/>
     <mergeCell ref="A30:A34"/>
@@ -4981,16 +5000,6 @@
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="F4:I4"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="O6:Q6"/>
-    <mergeCell ref="A10:A19"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:L6"/>
   </mergeCells>
   <conditionalFormatting sqref="M10:M41">
     <cfRule type="colorScale" priority="17">
@@ -23267,7 +23276,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:H5"/>
+  <dimension ref="B1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
@@ -23357,7 +23366,11 @@
         <v>33</v>
       </c>
     </row>
+    <row r="18" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="99"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>